<commit_message>
addig steps into Report view of swap to Duty manager persona script
</commit_message>
<xml_diff>
--- a/Data/WFMSwapToDutymangerPersonaTestData.xlsx
+++ b/Data/WFMSwapToDutymangerPersonaTestData.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8584C06E-06FD-43FB-B4A7-CF9F371EC638}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82D64064-BDE7-4D49-85F1-614AF9A620F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -458,7 +458,7 @@
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -538,7 +538,7 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError sqref="B1:E1 B4:C4 B2 D2 B3:C3 E3 E4" numberStoredAsText="1"/>
+    <ignoredError sqref="B1:E1 B4:C4 B2 B3:C3 E3 E4" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>